<commit_message>
610 Update classifier performance comparison
</commit_message>
<xml_diff>
--- a/resources/results/performance_comparison.xlsx
+++ b/resources/results/performance_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97AA634-65B3-9A4D-8276-C09D09D2841B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D3ED6-2931-B341-BD0D-4FD8DB8A93F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="2" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
@@ -1225,68 +1225,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0F12-3C43-93C8-983CE62493DF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet4!$E$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet4!$A$9:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>RF</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>RT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>IBk</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>LMT</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>MLP</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Auto-WEKA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet4!$E$9:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="6"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0F12-3C43-93C8-983CE62493DF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2680,15 +2618,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>910167</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>148167</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>105832</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3610,7 +3548,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
620 New testing set
</commit_message>
<xml_diff>
--- a/resources/results/performance_comparison.xlsx
+++ b/resources/results/performance_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairedeng/code/mirna/resources/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D3ED6-2931-B341-BD0D-4FD8DB8A93F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1486EE-D428-694F-BF7E-47E4805984FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="2" xr2:uid="{CE768B3B-9426-2340-8969-353CE113657E}"/>
   </bookViews>
@@ -477,16 +477,16 @@
     <t>LMT</t>
   </si>
   <si>
-    <t>Training Set</t>
-  </si>
-  <si>
-    <t>Testing Set 1 (18 miRNAs)</t>
-  </si>
-  <si>
-    <t>Testing Set 2 (20 miRNAs)</t>
-  </si>
-  <si>
     <t>Auto-WEKA</t>
+  </si>
+  <si>
+    <t>Training Dataset</t>
+  </si>
+  <si>
+    <t>Independent Dataset 1 [11]</t>
+  </si>
+  <si>
+    <t>Independent Dataset 2 [11]</t>
   </si>
 </sst>
 </file>
@@ -937,7 +937,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Tesing Sets (with CfsSubsetEval)</a:t>
+              <a:t> Independent Datasets (with CfsSubsetEval)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -988,7 +988,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Training Set</c:v>
+                  <c:v>Training Dataset</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1071,7 +1071,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Testing Set 1 (18 miRNAs)</c:v>
+                  <c:v>Independent Dataset 1 [11]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1154,7 +1154,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Testing Set 2 (20 miRNAs)</c:v>
+                  <c:v>Independent Dataset 2 [11]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3548,13 +3548,13 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
@@ -3612,13 +3612,13 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3698,7 +3698,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1">
         <v>0.99074099999999998</v>

</xml_diff>